<commit_message>
enable cell range for image insertion
</commit_message>
<xml_diff>
--- a/src/test/resources/test_files/working/InsertImage/valid_input.xlsx
+++ b/src/test/resources/test_files/working/InsertImage/valid_input.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28724"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://airarabia-my.sharepoint.com/personal/malhaq_isa_ae1/Documents/Documents/ExcelColumnConvert/ExcelColumnConvert/src/test/resources/test_files/working/InsertImage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://airarabia-my.sharepoint.com/personal/malhaq_isa_ae1/Documents/Documents/ExcelColumnConvert/ExcelColumnConvert/src/test/resources/test_files/originals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_74AC4085E3F66FFC05FC9890E22D62B1D0368FFE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BED777CD-CAC8-4781-9759-FC77E6829941}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_74AC4085E3F66FFC05FC9890E22D62B1D0368FFE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BB237DB-99F4-47B5-8B5E-7D7B3DEF86B1}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="28800" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="ad">Sheet1!$H$21</definedName>
-  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -114,7 +111,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,55 +163,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="533400" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,13 +454,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,7 +477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -546,7 +494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -563,7 +511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -580,7 +528,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -597,7 +545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -614,7 +562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -631,7 +579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -648,7 +596,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -665,7 +613,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -682,7 +630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -699,7 +647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -716,7 +664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -733,7 +681,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -750,7 +698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -767,7 +715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -784,7 +732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -801,7 +749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -818,7 +766,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -835,7 +783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -852,7 +800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -869,7 +817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -886,7 +834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -903,7 +851,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -920,7 +868,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -937,7 +885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -954,7 +902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -971,7 +919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -988,7 +936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1005,7 +953,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1022,7 +970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1039,7 +987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1056,7 +1004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1073,7 +1021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1096,6 +1044,5 @@
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Classification: External</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>